<commit_message>
login/ registration form 수정, context path 수정
</commit_message>
<xml_diff>
--- a/EnglishCat/doc/details.xlsx
+++ b/EnglishCat/doc/details.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\it\Documents\EnglishCat\EnglishCat\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D535E53-AE82-4139-A404-1C82079DBE58}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14415" windowHeight="9615" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14415" windowHeight="9615" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="메뉴 구성" sheetId="2" r:id="rId1"/>
@@ -21,7 +22,7 @@
     <sheet name="일지 (임시)" sheetId="8" r:id="rId7"/>
     <sheet name="메뉴 리스트" sheetId="1" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="223">
   <si>
     <t>잉글리쉬캣</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -944,11 +945,39 @@
 COMMENT ON COLUMN TB_CONT_REVIEW.DELETE_YN IS '삭제여부';</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>김대홍</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>현황 분석</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>joinform, loginform 틀 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TB_USER_INFO 테이블 및 컬럼 생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ovenapp 프로토타이핑 작성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>김대홍</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DB 환경 구축</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1339,7 +1368,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1622,7 +1651,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1707,14 +1736,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1825,14 +1854,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1980,7 +2009,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1988,7 +2017,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2415,7 +2444,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -2491,14 +2520,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2607,6 +2636,72 @@
         <v>124</v>
       </c>
     </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="8">
+        <v>43338</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="8">
+        <v>43339</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="8">
+        <v>43339</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="8">
+        <v>43340</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="8">
+        <v>43341</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="8">
+        <v>43341</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2615,7 +2710,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>

</xml_diff>